<commit_message>
add rank for the student
</commit_message>
<xml_diff>
--- a/student mark data.xlsx
+++ b/student mark data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29101"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01BEEFDA-156B-495F-BBE2-3B0F72660836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F3BAA49-8216-4C29-8E94-9D954F4B6BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,7 +556,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="K2" sqref="K2:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -640,7 +640,10 @@
         <f>AVERAGE(C2:H2)</f>
         <v>71.833333333333329</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2">
+        <f>RANK(I2,$I$2:$I$11)</f>
+        <v>4</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
@@ -677,7 +680,10 @@
         <f t="shared" ref="J3:J11" si="1">AVERAGE(C3:H3)</f>
         <v>79.5</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K11" si="2">RANK(I3,$I$2:$I$11)</f>
+        <v>2</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -714,7 +720,10 @@
         <f t="shared" si="1"/>
         <v>76.166666666666671</v>
       </c>
-      <c r="K4" s="2"/>
+      <c r="K4" s="2">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
@@ -751,7 +760,10 @@
         <f t="shared" si="1"/>
         <v>69.5</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
@@ -788,7 +800,10 @@
         <f t="shared" si="1"/>
         <v>53.833333333333336</v>
       </c>
-      <c r="K6" s="2"/>
+      <c r="K6" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
@@ -825,7 +840,10 @@
         <f t="shared" si="1"/>
         <v>41.333333333333336</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
@@ -862,7 +880,10 @@
         <f t="shared" si="1"/>
         <v>36.333333333333336</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
@@ -899,7 +920,10 @@
         <f t="shared" si="1"/>
         <v>31.333333333333332</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
@@ -936,7 +960,10 @@
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
@@ -973,7 +1000,10 @@
         <f t="shared" si="1"/>
         <v>95.833333333333329</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>

</xml_diff>